<commit_message>
Enhanced framework by organizing utils and pages.Scarped 800+ recipes for LFV Add
</commit_message>
<xml_diff>
--- a/Team06_CodeCrafters/src/test/resources/input_data/IngredientsAndComorbidities-ScrapperHackathon.xlsx
+++ b/Team06_CodeCrafters/src/test/resources/input_data/IngredientsAndComorbidities-ScrapperHackathon.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E0D0A7D8-B6FA-4762-B3C9-58B9124F1B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9638BA7F-5D3C-40EC-B65F-D5CAF4895E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30089,7 +30089,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="12.75">
       <c r="A3" s="18" t="s">
         <v>130</v>
       </c>
@@ -30106,7 +30106,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="12.75">
       <c r="A4" s="18" t="s">
         <v>135</v>
       </c>
@@ -30123,7 +30123,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="12.75">
       <c r="A5" s="18" t="s">
         <v>140</v>
       </c>
@@ -30138,7 +30138,7 @@
       </c>
       <c r="E5" s="18"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="12.75">
       <c r="A6" s="18" t="s">
         <v>144</v>
       </c>
@@ -30153,7 +30153,7 @@
       </c>
       <c r="E6" s="18"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="12.75">
       <c r="A7" s="18" t="s">
         <v>148</v>
       </c>
@@ -30166,7 +30166,7 @@
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="12.75">
       <c r="A8" s="18" t="s">
         <v>151</v>
       </c>
@@ -30180,7 +30180,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="12.75">
       <c r="A9" s="18" t="s">
         <v>154</v>
       </c>
@@ -30191,7 +30191,7 @@
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="12.75">
       <c r="A10" s="18" t="s">
         <v>156</v>
       </c>
@@ -30202,7 +30202,7 @@
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="12.75">
       <c r="A11" s="18" t="s">
         <v>158</v>
       </c>
@@ -30213,7 +30213,7 @@
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="12.75">
       <c r="A12" s="18" t="s">
         <v>160</v>
       </c>
@@ -30224,7 +30224,7 @@
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="12.75">
       <c r="A13" s="18" t="s">
         <v>162</v>
       </c>
@@ -30235,7 +30235,7 @@
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="12.75">
       <c r="A14" s="18" t="s">
         <v>164</v>
       </c>
@@ -30246,7 +30246,7 @@
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="12.75">
       <c r="A15" s="18" t="s">
         <v>166</v>
       </c>
@@ -30257,7 +30257,7 @@
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="12.75">
       <c r="A16" s="18" t="s">
         <v>168</v>
       </c>
@@ -30268,7 +30268,7 @@
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" ht="12.75">
       <c r="A17" s="18" t="s">
         <v>170</v>
       </c>
@@ -30279,7 +30279,7 @@
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" ht="12.75">
       <c r="A18" s="18" t="s">
         <v>172</v>
       </c>
@@ -30293,7 +30293,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" ht="12.75">
       <c r="A19" s="18" t="s">
         <v>175</v>
       </c>
@@ -30304,7 +30304,7 @@
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" ht="12.75">
       <c r="A20" s="18" t="s">
         <v>177</v>
       </c>
@@ -30315,7 +30315,7 @@
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" ht="12.75">
       <c r="A21" s="18" t="s">
         <v>179</v>
       </c>
@@ -31190,7 +31190,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" ht="12.75">
       <c r="A10" s="18" t="s">
         <v>165</v>
       </c>
@@ -31200,7 +31200,7 @@
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" ht="12.75">
       <c r="A11" s="18" t="s">
         <v>163</v>
       </c>
@@ -31210,7 +31210,7 @@
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" ht="12.75">
       <c r="A12" s="18" t="s">
         <v>322</v>
       </c>
@@ -31220,7 +31220,7 @@
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" ht="12.75">
       <c r="A13" s="18" t="s">
         <v>173</v>
       </c>
@@ -31230,7 +31230,7 @@
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="12.75">
       <c r="A14" s="18" t="s">
         <v>324</v>
       </c>
@@ -31240,7 +31240,7 @@
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="12.75">
       <c r="A15" s="18" t="s">
         <v>326</v>
       </c>
@@ -31250,7 +31250,7 @@
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" ht="12.75">
       <c r="A16" s="18" t="s">
         <v>328</v>
       </c>
@@ -31260,7 +31260,7 @@
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="12.75">
       <c r="A17" s="18" t="s">
         <v>330</v>
       </c>
@@ -31270,7 +31270,7 @@
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="12.75">
       <c r="A18" s="18" t="s">
         <v>332</v>
       </c>
@@ -31280,7 +31280,7 @@
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="12.75">
       <c r="A19" s="18" t="s">
         <v>334</v>
       </c>
@@ -31290,7 +31290,7 @@
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="12.75">
       <c r="A20" s="18" t="s">
         <v>335</v>
       </c>
@@ -31300,7 +31300,7 @@
       <c r="C20" s="18"/>
       <c r="D20" s="18"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="12.75">
       <c r="A21" s="18" t="s">
         <v>155</v>
       </c>
@@ -31937,67 +31937,67 @@
         <v>364</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" ht="12.75">
       <c r="A2" s="25" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" ht="12.75">
       <c r="A3" s="25" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" ht="12.75">
       <c r="A4" s="25" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" ht="12.75">
       <c r="A5" s="25" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" ht="12.75">
       <c r="A6" s="25" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" ht="12.75">
       <c r="A7" s="25" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" ht="12.75">
       <c r="A8" s="25" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" ht="12.75">
       <c r="A9" s="25" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" ht="12.75">
       <c r="A10" s="25" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" ht="12.75">
       <c r="A11" s="25" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" ht="12.75">
       <c r="A12" s="25" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" ht="12.75">
       <c r="A13" s="25" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" ht="12.75">
       <c r="A14" s="25" t="s">
         <v>370</v>
       </c>

</xml_diff>

<commit_message>
Updated LCHF and Ingredients xlsx
</commit_message>
<xml_diff>
--- a/Team06_CodeCrafters/src/test/resources/input_data/IngredientsAndComorbidities-ScrapperHackathon.xlsx
+++ b/Team06_CodeCrafters/src/test/resources/input_data/IngredientsAndComorbidities-ScrapperHackathon.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{9638BA7F-5D3C-40EC-B65F-D5CAF4895E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\limna\git\Team06_CodeCrafters\Team06_CodeCrafters\src\test\resources\input_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8578E6-A414-41AF-87F2-654E55864F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diabetes-Hypothyroidism-Hyperte" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,6 @@
     <sheet name="Filter -1 Allergies - Bonus Poi" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:D2"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="v4SQU0p9Lks/GIuIq3hSaF5r68xYc57Vk9JxVhlTvUo="/>
@@ -947,48 +951,27 @@
     <t>Processed Foods</t>
   </si>
   <si>
-    <t>1.       Raw,</t>
-  </si>
-  <si>
     <t>sausage</t>
   </si>
   <si>
-    <t>2.       Steamed,</t>
-  </si>
-  <si>
     <t>tinned fish</t>
   </si>
   <si>
     <t>poultry</t>
   </si>
   <si>
-    <t>3.       Boiled</t>
-  </si>
-  <si>
     <t>tuna</t>
   </si>
   <si>
-    <t>4.       Porched,</t>
-  </si>
-  <si>
     <t>Onion</t>
   </si>
   <si>
-    <t>5.       Sauted,</t>
-  </si>
-  <si>
-    <t>6.       Airfryed,</t>
-  </si>
-  <si>
     <t>beets</t>
   </si>
   <si>
     <t>turmeric</t>
   </si>
   <si>
-    <t>7.       Pan fried</t>
-  </si>
-  <si>
     <t>Ginger</t>
   </si>
   <si>
@@ -1137,6 +1120,27 @@
   </si>
   <si>
     <t>Seafood</t>
+  </si>
+  <si>
+    <t>Raw</t>
+  </si>
+  <si>
+    <t>Steamed</t>
+  </si>
+  <si>
+    <t>Boiled</t>
+  </si>
+  <si>
+    <t>Porched</t>
+  </si>
+  <si>
+    <t>Sauted</t>
+  </si>
+  <si>
+    <t>Airfryed</t>
+  </si>
+  <si>
+    <t>Pan fried</t>
   </si>
 </sst>
 </file>
@@ -30047,7 +30051,7 @@
   </sheetPr>
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
@@ -31072,7 +31076,9 @@
   </sheetPr>
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -31115,43 +31121,43 @@
         <v>306</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>307</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>170</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="24" t="s">
-        <v>309</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="18" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="24" t="s">
-        <v>312</v>
+        <v>366</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>168</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="24" t="s">
-        <v>314</v>
+        <v>367</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
@@ -31159,11 +31165,11 @@
         <v>150</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="24" t="s">
-        <v>316</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
@@ -31175,19 +31181,19 @@
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="24" t="s">
-        <v>317</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
       <c r="A9" s="18" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="24" t="s">
-        <v>320</v>
+        <v>370</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12.75">
@@ -31195,7 +31201,7 @@
         <v>165</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -31212,7 +31218,7 @@
     </row>
     <row r="12" spans="1:4" ht="12.75">
       <c r="A12" s="18" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>137</v>
@@ -31225,64 +31231,64 @@
         <v>173</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:4" ht="12.75">
       <c r="A14" s="18" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:4" ht="12.75">
       <c r="A15" s="18" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
     </row>
     <row r="16" spans="1:4" ht="12.75">
       <c r="A16" s="18" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
     </row>
     <row r="17" spans="1:4" ht="12.75">
       <c r="A17" s="18" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
     </row>
     <row r="18" spans="1:4" ht="12.75">
       <c r="A18" s="18" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
     </row>
     <row r="19" spans="1:4" ht="12.75">
       <c r="A19" s="18" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>288</v>
@@ -31292,7 +31298,7 @@
     </row>
     <row r="20" spans="1:4" ht="12.75">
       <c r="A20" s="18" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>290</v>
@@ -31312,7 +31318,7 @@
     </row>
     <row r="22" spans="1:4" ht="12.75">
       <c r="A22" s="18" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B22" s="18" t="s">
         <v>292</v>
@@ -31322,7 +31328,7 @@
     </row>
     <row r="23" spans="1:4" ht="12.75">
       <c r="A23" s="18" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>293</v>
@@ -31332,7 +31338,7 @@
     </row>
     <row r="24" spans="1:4" ht="12.75">
       <c r="A24" s="18" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>294</v>
@@ -31342,7 +31348,7 @@
     </row>
     <row r="25" spans="1:4" ht="12.75">
       <c r="A25" s="18" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>295</v>
@@ -31352,7 +31358,7 @@
     </row>
     <row r="26" spans="1:4" ht="12.75">
       <c r="A26" s="18" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>296</v>
@@ -31362,7 +31368,7 @@
     </row>
     <row r="27" spans="1:4" ht="12.75">
       <c r="A27" s="18" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>298</v>
@@ -31372,17 +31378,17 @@
     </row>
     <row r="28" spans="1:4" ht="12.75">
       <c r="A28" s="18" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
     </row>
     <row r="29" spans="1:4" ht="12.75">
       <c r="A29" s="18" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>300</v>
@@ -31392,7 +31398,7 @@
     </row>
     <row r="30" spans="1:4" ht="12.75">
       <c r="A30" s="18" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>301</v>
@@ -31402,7 +31408,7 @@
     </row>
     <row r="31" spans="1:4" ht="12.75">
       <c r="A31" s="18" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>302</v>
@@ -31412,37 +31418,37 @@
     </row>
     <row r="32" spans="1:4" ht="12.75">
       <c r="A32" s="18" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
     </row>
     <row r="33" spans="1:4" ht="12.75">
       <c r="A33" s="18" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
     </row>
     <row r="34" spans="1:4" ht="12.75">
       <c r="A34" s="18" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
     </row>
     <row r="35" spans="1:4" ht="12.75">
       <c r="A35" s="18" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
@@ -31450,7 +31456,7 @@
     </row>
     <row r="36" spans="1:4" ht="12.75">
       <c r="A36" s="18" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="B36" s="18"/>
       <c r="C36" s="18"/>
@@ -31458,7 +31464,7 @@
     </row>
     <row r="37" spans="1:4" ht="12.75">
       <c r="A37" s="18" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -31466,7 +31472,7 @@
     </row>
     <row r="38" spans="1:4" ht="12.75">
       <c r="A38" s="18" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="18"/>
@@ -31474,7 +31480,7 @@
     </row>
     <row r="39" spans="1:4" ht="12.75">
       <c r="A39" s="18" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="B39" s="18"/>
       <c r="C39" s="18"/>
@@ -31498,7 +31504,7 @@
     </row>
     <row r="42" spans="1:4" ht="12.75">
       <c r="A42" s="18" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="B42" s="18"/>
       <c r="C42" s="18"/>
@@ -31506,7 +31512,7 @@
     </row>
     <row r="43" spans="1:4" ht="12.75">
       <c r="A43" s="18" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="B43" s="18"/>
       <c r="C43" s="18"/>
@@ -31514,7 +31520,7 @@
     </row>
     <row r="44" spans="1:4" ht="12.75">
       <c r="A44" s="18" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="B44" s="18"/>
       <c r="C44" s="18"/>
@@ -31778,7 +31784,7 @@
     </row>
     <row r="77" spans="1:4" ht="12.75">
       <c r="A77" s="18" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="B77" s="18"/>
       <c r="C77" s="18"/>
@@ -31882,7 +31888,7 @@
     </row>
     <row r="90" spans="1:4" ht="12.75">
       <c r="A90" s="18" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="B90" s="18"/>
       <c r="C90" s="18"/>
@@ -31890,7 +31896,7 @@
     </row>
     <row r="91" spans="1:4" ht="12.75">
       <c r="A91" s="18" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="B91" s="18"/>
       <c r="C91" s="18"/>
@@ -31898,7 +31904,7 @@
     </row>
     <row r="92" spans="1:4" ht="12.75">
       <c r="A92" s="18" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="B92" s="18"/>
       <c r="C92" s="18"/>
@@ -31934,27 +31940,27 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1">
       <c r="A1" s="17" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="12.75">
       <c r="A2" s="25" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="12.75">
       <c r="A3" s="25" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="12.75">
       <c r="A4" s="25" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="12.75">
       <c r="A5" s="25" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="12.75">
@@ -31994,12 +32000,12 @@
     </row>
     <row r="13" spans="1:1" ht="12.75">
       <c r="A13" s="25" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="12.75">
       <c r="A14" s="25" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>